<commit_message>
made a new file and changed data values a bit
</commit_message>
<xml_diff>
--- a/data/stock_data/S&P500_data.xlsx
+++ b/data/stock_data/S&P500_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/Documents/code/Research-Project/data/stock_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFC83DBD-2203-FD42-925C-37446D5EF26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2A0039-01AB-0848-9E00-4483DAE5517C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37440" yWindow="-12020" windowWidth="28480" windowHeight="16440" xr2:uid="{E8AD4466-DECB-074F-90C9-6F2E91701384}"/>
   </bookViews>
@@ -53,13 +53,13 @@
     <t>Close*</t>
   </si>
   <si>
-    <t>Up / Down</t>
-  </si>
-  <si>
     <t>Avg. Sentiment Score</t>
   </si>
   <si>
     <t>Avg. Stock Price</t>
+  </si>
+  <si>
+    <t>Tragectory</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,13 +596,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
made a linear regression model
</commit_message>
<xml_diff>
--- a/data/stock_data/S&P500_data.xlsx
+++ b/data/stock_data/S&P500_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/Documents/code/Research-Project/data/stock_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2A0039-01AB-0848-9E00-4483DAE5517C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838EB1CF-DAB7-6743-A83A-8B6399508B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37440" yWindow="-12020" windowWidth="28480" windowHeight="16440" xr2:uid="{E8AD4466-DECB-074F-90C9-6F2E91701384}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J3"/>
+      <selection activeCell="I16" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,7 +622,7 @@
         <v>4396.4399999999996</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F22" si="0" xml:space="preserve"> (B2+C2+D2+E2)/4</f>
+        <f xml:space="preserve"> (B2+C2+D2+E2)/4</f>
         <v>4385.4349999999995</v>
       </c>
       <c r="G2">
@@ -649,7 +649,7 @@
         <v>4450.38</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B3+C3+D3+E3)/4</f>
         <v>4438.4349999999995</v>
       </c>
       <c r="G3">
@@ -677,7 +677,7 @@
         <v>4455.59</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B4+C4+D4+E4)/4</f>
         <v>4451.2049999999999</v>
       </c>
       <c r="G4">
@@ -705,7 +705,7 @@
         <v>4446.82</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B5+C5+D5+E5)/4</f>
         <v>4444.8824999999997</v>
       </c>
       <c r="G5">
@@ -733,7 +733,7 @@
         <v>4411.59</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B6+C6+D6+E6)/4</f>
         <v>4410.47</v>
       </c>
       <c r="G6">
@@ -761,7 +761,7 @@
         <v>4398.95</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B7+C7+D7+E7)/4</f>
         <v>4410.32</v>
       </c>
       <c r="G7">
@@ -789,7 +789,7 @@
         <v>4409.53</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B8+C8+D8+E8)/4</f>
         <v>4401.57</v>
       </c>
       <c r="G8">
@@ -817,7 +817,7 @@
         <v>4439.26</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B9+C9+D9+E9)/4</f>
         <v>4426.7275000000009</v>
       </c>
       <c r="G9">
@@ -845,7 +845,7 @@
         <v>4472.16</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B10+C10+D10+E10)/4</f>
         <v>4472.8549999999996</v>
       </c>
       <c r="G10">
@@ -873,7 +873,7 @@
         <v>4510.04</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B11+C11+D11+E11)/4</f>
         <v>4502.0700000000006</v>
       </c>
       <c r="G11">
@@ -901,7 +901,7 @@
         <v>4505.42</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B12+C12+D12+E12)/4</f>
         <v>4511.8374999999996</v>
       </c>
       <c r="G12">
@@ -929,7 +929,7 @@
         <v>4522.79</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B13+C13+D13+E13)/4</f>
         <v>4517.3499999999995</v>
       </c>
       <c r="G13">
@@ -957,7 +957,7 @@
         <v>4554.9799999999996</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B14+C14+D14+E14)/4</f>
         <v>4538.4125000000004</v>
       </c>
       <c r="G14">
@@ -985,7 +985,7 @@
         <v>4565.72</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B15+C15+D15+E15)/4</f>
         <v>4566.375</v>
       </c>
       <c r="G15">
@@ -1013,7 +1013,7 @@
         <v>4534.87</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B16+C16+D16+E16)/4</f>
         <v>4545.3874999999998</v>
       </c>
       <c r="G16">
@@ -1041,7 +1041,7 @@
         <v>4536.34</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B17+C17+D17+E17)/4</f>
         <v>4544.3225000000002</v>
       </c>
       <c r="G17">
@@ -1069,7 +1069,7 @@
         <v>4554.6400000000003</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B18+C18+D18+E18)/4</f>
         <v>4550.6824999999999</v>
       </c>
       <c r="G18">
@@ -1097,7 +1097,7 @@
         <v>4567.46</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B19+C19+D19+E19)/4</f>
         <v>4563.9224999999997</v>
       </c>
       <c r="G19">
@@ -1125,7 +1125,7 @@
         <v>4566.75</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B20+C20+D20+E20)/4</f>
         <v>4563.9400000000005</v>
       </c>
       <c r="G20">
@@ -1153,7 +1153,7 @@
         <v>4537.41</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B21+C21+D21+E21)/4</f>
         <v>4567.8249999999998</v>
       </c>
       <c r="G21">
@@ -1181,14 +1181,14 @@
         <v>4582.2299999999996</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
+        <f xml:space="preserve"> (B22+C22+D22+E22)/4</f>
         <v>4575.5375000000004</v>
       </c>
       <c r="G22">
         <v>0.57499999999999996</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" ref="H22:H23" si="1" xml:space="preserve"> IF(F21&lt;F22,1,0)</f>
+        <f xml:space="preserve"> IF(F21&lt;F22,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
+        <f xml:space="preserve"> IF(F22&lt;F23,1,0)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>